<commit_message>
added WSC article and some style changes
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Description</t>
   </si>
@@ -51,6 +51,21 @@
   </si>
   <si>
     <t>give-a-gift-article</t>
+  </si>
+  <si>
+    <t>article-3.html</t>
+  </si>
+  <si>
+    <t>365 Days as an exchange student</t>
+  </si>
+  <si>
+    <t>article-4.html</t>
+  </si>
+  <si>
+    <t>World Scholar's Cup</t>
+  </si>
+  <si>
+    <t>article-5.html</t>
   </si>
 </sst>
 </file>
@@ -388,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,6 +449,27 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added romnea pisei article
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Description</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>article-5.html</t>
+  </si>
+  <si>
+    <t>Music Fair</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,7 +457,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -468,6 +471,9 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added mona article corona
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Description</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Music Fair</t>
+  </si>
+  <si>
+    <t>article-6.html</t>
+  </si>
+  <si>
+    <t>How Are WIS students coping with this new Pandemic?</t>
   </si>
 </sst>
 </file>
@@ -406,7 +412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -415,7 +421,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.21875" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="2" max="2" width="48.44140625" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
@@ -476,6 +482,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>